<commit_message>
Master v2 - WIP
</commit_message>
<xml_diff>
--- a/abbreviation_llm.xlsx
+++ b/abbreviation_llm.xlsx
@@ -3167,7 +3167,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B207"/>
+  <dimension ref="A1:B205"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3188,7 +3188,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>École Polytechnique de l'Ouest de la Guinée</t>
+          <t>Ecole Polytechnique de l'Ouest de la Guinée</t>
         </is>
       </c>
     </row>
@@ -3236,7 +3236,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Institut des Sciences et Techniques de la Communication</t>
+          <t>Institut des Stratégies et Techniques de Communication</t>
         </is>
       </c>
     </row>
@@ -3248,7 +3248,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Concours d'Accès au Corps des Professeurs de l'Enseignement Privé</t>
+          <t>Concours d'Accès au Corps des Formateurs de Personnels</t>
         </is>
       </c>
     </row>
@@ -3332,7 +3332,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Institut National de Perfectionnement et d'Éducation des Enseignants</t>
+          <t>Institut National de Perfectionnement et d'Éducateurs</t>
         </is>
       </c>
     </row>
@@ -3368,7 +3368,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>École Supérieure des Sciences du Langage, de l'Information et de la Communication</t>
+          <t>École Supérieure des Sciences et Langues pour l'Ingénieur de Lille</t>
         </is>
       </c>
     </row>
@@ -3392,7 +3392,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>École Nationale des Langues et Civilisations de l'Orient</t>
+          <t>...</t>
         </is>
       </c>
     </row>
@@ -3632,7 +3632,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Licence de Langues, Littératures et Civilisations Étrangères</t>
+          <t>Licence Langues, Littératures et Civilisations Étrangères et Régionales</t>
         </is>
       </c>
     </row>
@@ -3668,7 +3668,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Éducation Morale et Civique</t>
+          <t>École de Management de la Chambre de Commerce et d'Industrie de Paris</t>
         </is>
       </c>
     </row>
@@ -3848,7 +3848,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Université des Sciences et Technologies de Hanoï</t>
+          <t>Université de Science et Technologie de Hanoï</t>
         </is>
       </c>
     </row>
@@ -3968,7 +3968,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Université Internationale</t>
+          <t>...</t>
         </is>
       </c>
     </row>
@@ -4076,7 +4076,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Sciences Humaines et Politiques Sociales</t>
+          <t>Sciences Humaines et Sociales, Philosophie, Sociologie</t>
         </is>
       </c>
     </row>
@@ -5300,7 +5300,7 @@
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>...</t>
+          <t>Diplôme Universitaire de Musicien Intervenant</t>
         </is>
       </c>
     </row>
@@ -5372,7 +5372,7 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>...</t>
+          <t>Sciences Humaines et Sociales, Philosophie</t>
         </is>
       </c>
     </row>
@@ -5516,7 +5516,7 @@
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>...</t>
+          <t>Institut Supérieur de Formation de l'Enseignement Catholique</t>
         </is>
       </c>
     </row>
@@ -5622,31 +5622,7 @@
           <t>DSP</t>
         </is>
       </c>
-      <c r="B205" t="inlineStr">
-        <is>
-          <t>...</t>
-        </is>
-      </c>
-    </row>
-    <row r="206">
-      <c r="A206" s="1" t="inlineStr">
-        <is>
-          <t>UPPA</t>
-        </is>
-      </c>
-      <c r="B206" t="inlineStr">
-        <is>
-          <t>Université de Pau et des Pays de l'Adour</t>
-        </is>
-      </c>
-    </row>
-    <row r="207">
-      <c r="A207" s="1" t="inlineStr">
-        <is>
-          <t>SCM</t>
-        </is>
-      </c>
-      <c r="B207" t="inlineStr"/>
+      <c r="B205" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>